<commit_message>
Finished clue layout with test plans as well as all target tests
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTestPlanning.xlsx
+++ b/data/ClueLayoutTestPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spect\eclipse-workspace\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62E4DD1-ABD1-442D-B07E-2706719A8B18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837BBCD-923A-4708-B294-4EE6804A3314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -258,15 +258,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,11 +287,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -386,12 +374,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -405,32 +392,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -707,7 +690,7 @@
   <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -716,7 +699,7 @@
     <col min="29" max="29" width="78.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>0</v>
@@ -798,7 +781,7 @@
       </c>
       <c r="AC1" s="8"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -881,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -967,7 +950,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1031,7 +1014,7 @@
       <c r="U4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="V4" s="24" t="s">
         <v>4</v>
       </c>
       <c r="W4" s="4" t="s">
@@ -1053,7 +1036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1136,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1222,7 +1205,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1308,7 +1291,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1394,7 +1377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1480,7 +1463,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1563,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1646,7 +1629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1729,7 +1712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1812,7 +1795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1895,7 +1878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1978,7 +1961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2061,7 +2044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2144,7 +2127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2226,14 +2209,14 @@
       <c r="AA18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC18" s="24" t="s">
+      <c r="AC18" s="22" t="s">
         <v>43</v>
       </c>
       <c r="AD18" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2267,7 +2250,7 @@
       <c r="K19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="19" t="s">
         <v>2</v>
       </c>
       <c r="M19" s="21" t="s">
@@ -2315,14 +2298,14 @@
       <c r="AA19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AC19" s="25" t="s">
+      <c r="AC19" s="23" t="s">
         <v>44</v>
       </c>
       <c r="AD19" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2404,14 +2387,14 @@
       <c r="AA20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC20" s="25" t="s">
+      <c r="AC20" s="23" t="s">
         <v>45</v>
       </c>
       <c r="AD20" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2493,14 +2476,14 @@
       <c r="AA21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC21" s="25" t="s">
+      <c r="AC21" s="23" t="s">
         <v>46</v>
       </c>
       <c r="AD21" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2582,14 +2565,14 @@
       <c r="AA22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC22" s="25" t="s">
+      <c r="AC22" s="23" t="s">
         <v>47</v>
       </c>
       <c r="AD22" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2671,14 +2654,14 @@
       <c r="AA23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC23" s="25" t="s">
+      <c r="AC23" s="23" t="s">
         <v>48</v>
       </c>
       <c r="AD23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2760,9 +2743,9 @@
       <c r="AA24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC24" s="23"/>
+      <c r="AC24" s="25"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2844,14 +2827,14 @@
       <c r="AA25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC25" s="25" t="s">
+      <c r="AC25" s="23" t="s">
         <v>54</v>
       </c>
       <c r="AD25" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2933,14 +2916,14 @@
       <c r="AA26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC26" s="22" t="s">
+      <c r="AC26" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AD26" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -3022,14 +3005,14 @@
       <c r="AA27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC27" s="22" t="s">
+      <c r="AC27" s="23" t="s">
         <v>56</v>
       </c>
       <c r="AD27" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -3111,7 +3094,7 @@
       <c r="AA28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AC28" s="22" t="s">
+      <c r="AC28" s="23" t="s">
         <v>57</v>
       </c>
       <c r="AD28" s="4" t="s">
@@ -3119,7 +3102,7 @@
       </c>
     </row>
     <row r="29" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AC29" s="22" t="s">
+      <c r="AC29" s="23" t="s">
         <v>58</v>
       </c>
       <c r="AD29" s="4" t="s">
@@ -3127,32 +3110,32 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&gt;">
       <formula>NOT(ISERROR(SEARCH(("&gt;"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH(("&lt;"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="^">
       <formula>NOT(ISERROR(SEARCH(("^"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:L19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
     <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="v">
       <formula>NOT(ISERROR(SEARCH(("v"),(B2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed BoardAdjTargetTest.java tests to test for the correct things. All tests in the tests package now pass.
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTestPlanning.xlsx
+++ b/data/ClueLayoutTestPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spect\eclipse-workspace\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837BBCD-923A-4708-B294-4EE6804A3314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9928B994-1B49-46E7-A95D-CCD456BD7FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,151 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -690,7 +834,7 @@
   <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC32" sqref="AC32"/>
+      <selection activeCell="N20" activeCellId="5" sqref="J18 I19 J20 L20 K19 N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1244,7 @@
       <c r="U5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="W5" s="4" t="s">
@@ -1859,7 +2003,7 @@
       <c r="U14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="V14" s="10" t="s">
         <v>23</v>
       </c>
       <c r="W14" s="4" t="s">
@@ -3110,39 +3254,69 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&gt;">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="&gt;">
       <formula>NOT(ISERROR(SEARCH(("&gt;"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH(("&lt;"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="^">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="^">
       <formula>NOT(ISERROR(SEARCH(("^"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B3:AA6 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B10:AA17 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29">
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="v">
+  <conditionalFormatting sqref="AC3:AC4 AC6:AC9 B28:Q28 S28:AA28 B20:AA22 B19:K19 B8:Y8 C7:AA7 B2:H2 J2:AA2 B18:V18 X18:AA18 B9:M9 O9:AA9 AD18:AD23 AA8 B24:AA27 B23:Q23 S23:AA23 N19:Z19 AD25:AD29 B6:AA6 B5:U5 W5:AA5 B3:AA4 B10:AA17">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="v">
       <formula>NOT(ISERROR(SEARCH(("v"),(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC16">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19">
       <formula>LEN(TRIM(AC16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="&gt;">
+      <formula>NOT(ISERROR(SEARCH(("&gt;"),(V5))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH(("&lt;"),(V5))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="^">
+      <formula>NOT(ISERROR(SEARCH(("^"),(V5))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="v">
+      <formula>NOT(ISERROR(SEARCH(("v"),(V5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>